<commit_message>
results for subclasses added
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2137kg/lab/thesis/extended/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD26B6B-632D-CD4E-A297-A82CF7CD2CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64426650-CDCA-094D-8FED-AC92D1502229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15920" xr2:uid="{54A87FC7-399E-024A-B748-A349380E7345}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15920" activeTab="1" xr2:uid="{54A87FC7-399E-024A-B748-A349380E7345}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="first_experiments" sheetId="1" r:id="rId1"/>
+    <sheet name="5-sub classes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>entropy</t>
   </si>
@@ -64,6 +65,12 @@
   </si>
   <si>
     <t>1ラベル</t>
+  </si>
+  <si>
+    <t>全クラス使った</t>
+  </si>
+  <si>
+    <t>乱数で選んだ5クラスだけ使った</t>
   </si>
 </sst>
 </file>
@@ -168,41 +175,41 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,99 +525,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892600A5-9E9B-7040-9AB6-4AC46A105B05}">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="17" x14ac:dyDescent="0.15">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>81.679999999999893</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>27.279999999999902</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <v>4.93</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="17" x14ac:dyDescent="0.15">
-      <c r="B5" s="3"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>79.869999999999905</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>27.189999999999898</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="17" x14ac:dyDescent="0.15">
-      <c r="B6" s="3"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>45.4</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>27.27</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>4.7300000000000004</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="17" x14ac:dyDescent="0.15">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>86.02</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>28.96</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>7.72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B4:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688FD77A-EC1E-2541-85AC-0B951B03934A}">
+  <dimension ref="B2:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>84.11</v>
+      </c>
+      <c r="E4" s="6">
+        <v>42.42</v>
+      </c>
+      <c r="F4" s="8">
+        <v>20.59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B5" s="12"/>
+      <c r="C5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>81.180000000000007</v>
+      </c>
+      <c r="E5" s="6">
+        <v>41.18</v>
+      </c>
+      <c r="F5" s="9">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B6" s="12"/>
+      <c r="C6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>66.03</v>
+      </c>
+      <c r="E6" s="6">
+        <v>39.24</v>
+      </c>
+      <c r="F6" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7">
+        <v>85.97</v>
+      </c>
+      <c r="E7" s="7">
+        <v>40.520000000000003</v>
+      </c>
+      <c r="F7" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>